<commit_message>
Corrigindo footprint dos jacks RCA Corrigindo lista de peças da revisão 7
</commit_message>
<xml_diff>
--- a/Rev7/Docs/BOM.xlsx
+++ b/Rev7/Docs/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>PCB TK90X - Rev 7</t>
   </si>
@@ -246,13 +246,25 @@
   </si>
   <si>
     <t>AV-8.4-3, Keystone 589/938 or PDI RCA-061X-Y</t>
+  </si>
+  <si>
+    <t>OBSERVAÇÕES</t>
+  </si>
+  <si>
+    <t>Se for montar com 32K de RAM alta, reduzir um</t>
+  </si>
+  <si>
+    <t>resistor de 1K (comprar somente 5) e reduzir dois</t>
+  </si>
+  <si>
+    <t>diodos 1N4148 (comprar somente 22)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,13 +288,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -297,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -316,6 +341,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,10 +952,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="8">
         <v>24</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1098,6 +1132,10 @@
       <c r="B35" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E35" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -1106,6 +1144,10 @@
       <c r="B36" s="4">
         <v>75</v>
       </c>
+      <c r="E36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -1114,6 +1156,10 @@
       <c r="B37" s="4">
         <v>100</v>
       </c>
+      <c r="E37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -1122,6 +1168,10 @@
       <c r="B38" s="4">
         <v>150</v>
       </c>
+      <c r="E38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -1148,10 +1198,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="8">
         <v>6</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1173,7 +1223,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>32</v>

</xml_diff>